<commit_message>
edit 8/21 add STD
</commit_message>
<xml_diff>
--- a/table_plan.xlsx
+++ b/table_plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,20 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="2" r:id="rId1"/>
     <sheet name="shop" sheetId="3" r:id="rId2"/>
     <sheet name="menu" sheetId="10" r:id="rId3"/>
-    <sheet name="like" sheetId="11" r:id="rId4"/>
-    <sheet name="holiday" sheetId="4" r:id="rId5"/>
-    <sheet name="closest_station" sheetId="12" r:id="rId6"/>
+    <sheet name="holiday" sheetId="4" r:id="rId4"/>
+    <sheet name="holiday_ex" sheetId="14" r:id="rId5"/>
+    <sheet name="keywords" sheetId="8" r:id="rId6"/>
     <sheet name="station" sheetId="13" r:id="rId7"/>
-    <sheet name="keywords" sheetId="8" r:id="rId8"/>
+    <sheet name="line" sheetId="15" r:id="rId8"/>
     <sheet name="review" sheetId="5" r:id="rId9"/>
-    <sheet name="favorite" sheetId="7" r:id="rId10"/>
-    <sheet name="pictures" sheetId="9" r:id="rId11"/>
+    <sheet name="pictures" sheetId="9" r:id="rId10"/>
+    <sheet name="scene" sheetId="18" r:id="rId11"/>
+    <sheet name="like" sheetId="11" r:id="rId12"/>
+    <sheet name="favorite" sheetId="7" r:id="rId13"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="160">
   <si>
     <t>物理名</t>
     <rPh sb="0" eb="3">
@@ -399,13 +401,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>駅名</t>
-    <rPh sb="0" eb="2">
-      <t>エキメ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ユーザ名</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -441,10 +436,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>user_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>int unsigned</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -495,25 +486,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>class</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>varchar</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>smallint unsigned</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>外人考慮</t>
-    <rPh sb="0" eb="2">
-      <t>ガイジn</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>コウry</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -596,16 +573,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>物理削除と論理削除</t>
-    <rPh sb="0" eb="4">
-      <t>ブツr</t>
-    </rPh>
-    <rPh sb="5" eb="9">
-      <t>ロンリサク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>論理削除か物理削除か</t>
     <rPh sb="0" eb="4">
       <t>ロンr</t>
@@ -654,26 +621,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>更新数が一番大きい？</t>
-    <rPh sb="0" eb="3">
-      <t>コウシn</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>イチバn</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>オオキ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>フラグを立てる？</t>
-    <rPh sb="4" eb="5">
-      <t>タt</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>編集をすると最大更新数＋１でレコードが挿入される。</t>
     <rPh sb="0" eb="2">
       <t>ヘンシュ</t>
@@ -710,38 +657,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>nearest_station</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>駅ID</t>
-    <rPh sb="0" eb="1">
-      <t>エキメ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>station_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>修正日</t>
   </si>
   <si>
     <t>modified</t>
-  </si>
-  <si>
-    <t>編集する時は駅IDを更新する</t>
-    <rPh sb="0" eb="2">
-      <t>ヘンシュ</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>エk</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>コウシn</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>沿線</t>
@@ -757,32 +676,6 @@
     <t>created</t>
   </si>
   <si>
-    <t>line</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>番号</t>
-    <rPh sb="0" eb="2">
-      <t>バンゴ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>キーワード番号</t>
-    <rPh sb="5" eb="7">
-      <t>バンゴ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1~5</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ロックかける必要なし</t>
     <rPh sb="6" eb="8">
       <t>ヒツヨ</t>
@@ -803,22 +696,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>フラグ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>flag</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1 or 2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2だとお気に入り</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>１ユーザ１店舗につき５枚より多く登録できない</t>
     <rPh sb="14" eb="15">
       <t>オオk</t>
@@ -835,6 +712,292 @@
     </rPh>
     <rPh sb="12" eb="13">
       <t>モタn</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>日付</t>
+    <rPh sb="0" eb="2">
+      <t>ヒヅk</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>holiday_ex</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PRI</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>UNIQ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>世代保持数</t>
+    <rPh sb="0" eb="5">
+      <t>セダ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>１〜７</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>versionをうまく使おう</t>
+    <rPh sb="11" eb="12">
+      <t>ツカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>varchar groupby重い</t>
+    <rPh sb="15" eb="16">
+      <t>オモ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>制御側でレコード制限</t>
+    <rPh sb="0" eb="3">
+      <t>セイgy</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>セイゲn</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>pictureも一緒</t>
+    <rPh sb="8" eb="10">
+      <t>イッsy</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>外国人考慮</t>
+    <rPh sb="0" eb="3">
+      <t>ガイコk</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>コウry</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sha256</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>division</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>復元できるように論理削除</t>
+    <rPh sb="0" eb="2">
+      <t>フクゲn</t>
+    </rPh>
+    <rPh sb="8" eb="12">
+      <t>ロンr</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>世代保持数５０？</t>
+    <rPh sb="0" eb="5">
+      <t>セダ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>最寄駅</t>
+    <rPh sb="0" eb="3">
+      <t>モヨr</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>station_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>休日ID</t>
+    <rPh sb="0" eb="2">
+      <t>キュ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>holiday_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>holiday_ex_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>休日例外ID</t>
+    <rPh sb="0" eb="2">
+      <t>キュ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>レイガ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>line_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>smallint unsign</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>station_name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>駅名</t>
+    <rPh sb="0" eb="2">
+      <t>エk</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>line</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>沿線名</t>
+    <rPh sb="0" eb="2">
+      <t>エンセn</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>メ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>line_name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>auto_increment</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>表示は作成日でorder by</t>
+    <rPh sb="0" eb="2">
+      <t>ヒョ</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>サクセ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>scene_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>tinyint unsigned</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>シーン名</t>
+    <rPh sb="3" eb="4">
+      <t>メ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>shopごとに作成日でorder by</t>
+    <rPh sb="7" eb="10">
+      <t>サクセ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>沿線ごとにIdで並べる。IDは実際の駅順でつける</t>
+    <rPh sb="0" eb="2">
+      <t>エンセンゴt</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ナラb</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ジッサ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>エk</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>name 分けなくていい</t>
+    <rPh sb="5" eb="6">
+      <t>ワケナクt</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>order_no</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メニューは全体一括更新</t>
+    <rPh sb="5" eb="7">
+      <t>ゼンタ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>イッk</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>コウシn</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ショップ、メニュー、休日それぞれで復元できるようにする。それぞれ独立した更新数を持っていて復元に使う。履歴はそれぞれ作る。それぞれ世代保持数は２０くらい？</t>
+    <rPh sb="10" eb="12">
+      <t>キュウジt</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>フクゲn</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ドクリt</t>
+    </rPh>
+    <rPh sb="36" eb="39">
+      <t>コウシn</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>モッt</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>フクゲn</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>リレk</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>ツクr</t>
+    </rPh>
+    <rPh sb="65" eb="67">
+      <t>セダ</t>
+    </rPh>
+    <rPh sb="67" eb="70">
+      <t>ホj</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -932,7 +1095,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -993,15 +1156,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -1026,7 +1180,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1042,18 +1196,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1062,6 +1216,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1075,21 +1239,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="19">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -1097,6 +1248,8 @@
     <cellStyle name="ハイパーリンク" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -1105,6 +1258,8 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="18" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1382,7 +1537,7 @@
   <dimension ref="B3:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
@@ -1395,15 +1550,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="16"/>
     </row>
     <row r="4" spans="2:10" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
@@ -1433,10 +1588,10 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E5" s="1">
         <v>5</v>
@@ -1449,7 +1604,7 @@
         <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="21" x14ac:dyDescent="0.35">
@@ -1457,7 +1612,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
@@ -1469,7 +1624,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="1"/>
       <c r="J6" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="21" x14ac:dyDescent="0.35">
@@ -1502,11 +1657,14 @@
         <v>9</v>
       </c>
       <c r="E8" s="1">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="1"/>
+      <c r="J8" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="9" spans="2:10" ht="21" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
@@ -1516,7 +1674,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -1525,23 +1683,23 @@
       <c r="G9" s="2"/>
       <c r="H9" s="1"/>
       <c r="J9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="21" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>88</v>
+        <v>133</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E10" s="1">
-        <v>10</v>
-      </c>
-      <c r="F10" s="9"/>
+        <v>20</v>
+      </c>
+      <c r="F10" s="7"/>
       <c r="G10" s="2"/>
       <c r="H10" s="1"/>
     </row>
@@ -1558,11 +1716,11 @@
       <c r="E11" s="1">
         <v>10</v>
       </c>
-      <c r="F11" s="9"/>
+      <c r="F11" s="7"/>
       <c r="G11" s="2"/>
       <c r="H11" s="1"/>
       <c r="J11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="21" x14ac:dyDescent="0.35">
@@ -1591,8 +1749,8 @@
         <v>14</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="9" t="s">
-        <v>77</v>
+      <c r="F13" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="1"/>
@@ -1608,32 +1766,31 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J20"/>
+  <dimension ref="B2:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
-    </row>
-    <row r="3" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1656,7 +1813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>38</v>
       </c>
@@ -1664,45 +1821,41 @@
         <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E4" s="1">
         <v>5</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>109</v>
-      </c>
+      <c r="G4" s="2"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="E5" s="1">
         <v>6</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
-        <v>109</v>
-      </c>
+      <c r="G5" s="2"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>134</v>
+        <v>74</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>97</v>
+        <v>152</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -1710,56 +1863,58 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="1"/>
-      <c r="I6" t="s">
-        <v>136</v>
-      </c>
-      <c r="J6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
+    </row>
+    <row r="7" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+    <row r="8" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="2"/>
+      <c r="F8" s="7"/>
       <c r="G8" s="2"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+    <row r="9" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="2"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="2"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1768,7 +1923,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1777,7 +1932,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1786,7 +1941,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1795,9 +1950,32 @@
       <c r="G14" s="2"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D20" t="s">
-        <v>106</v>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1811,30 +1989,31 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I20"/>
+  <dimension ref="B2:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
-    </row>
-    <row r="3" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1857,125 +2036,106 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>90</v>
+        <v>152</v>
       </c>
       <c r="E4" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
-        <v>109</v>
-      </c>
+      <c r="G5" s="2"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>128</v>
+        <v>75</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>129</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>97</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>109</v>
-      </c>
+      <c r="G6" s="2"/>
       <c r="H6" s="1"/>
-      <c r="I6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1">
-        <v>10</v>
-      </c>
-      <c r="F7" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1">
-        <v>255</v>
-      </c>
-      <c r="F8" s="9"/>
+    <row r="8" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="7"/>
       <c r="G8" s="2"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B9" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>14</v>
-      </c>
+    <row r="9" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="9"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="2"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1984,7 +2144,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1993,7 +2153,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2002,7 +2162,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2011,27 +2171,351 @@
       <c r="G14" s="2"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D17" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D18" t="s">
-        <v>139</v>
-      </c>
-      <c r="G18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="G19" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="G20" t="s">
-        <v>108</v>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H2"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B8" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B9" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H2"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:H20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2045,10 +2529,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H23"/>
+  <dimension ref="B3:H26"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
@@ -2060,15 +2544,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
+      <c r="B3" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="16"/>
     </row>
     <row r="4" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
@@ -2098,7 +2582,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>47</v>
@@ -2108,7 +2592,7 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2117,13 +2601,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="1">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2139,8 +2623,8 @@
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="6">
-        <v>30</v>
+      <c r="E7" s="4">
+        <v>100</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2151,13 +2635,13 @@
         <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>50</v>
       </c>
       <c r="E8" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2173,7 +2657,7 @@
       <c r="D9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>49</v>
       </c>
       <c r="F9" s="2"/>
@@ -2188,12 +2672,12 @@
         <v>57</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E10" s="1">
         <v>5</v>
       </c>
-      <c r="F10" s="9"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="2"/>
       <c r="H10" s="1"/>
     </row>
@@ -2210,22 +2694,22 @@
       <c r="E11" s="1">
         <v>255</v>
       </c>
-      <c r="F11" s="9"/>
+      <c r="F11" s="7"/>
       <c r="G11" s="2"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
-        <v>56</v>
+        <v>136</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>79</v>
+        <v>137</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E12" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -2233,85 +2717,99 @@
     </row>
     <row r="13" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E13" s="1">
-        <v>10</v>
-      </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="2" t="s">
-        <v>109</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="1">
         <v>10</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="9" t="s">
-        <v>77</v>
-      </c>
+      <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="19" spans="2:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="B19" s="7"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="18" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="C18" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F22" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F23" t="s">
-        <v>114</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>125</v>
+      </c>
+      <c r="E26" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2325,10 +2823,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H16"/>
+  <dimension ref="B2:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:H13"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
@@ -2340,15 +2838,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
@@ -2378,36 +2876,36 @@
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E5" s="1">
         <v>6</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2436,7 +2934,7 @@
         <v>63</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E7" s="1">
         <v>5</v>
@@ -2447,19 +2945,21 @@
     </row>
     <row r="8" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E8" s="1">
         <v>10</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="2:8" ht="21" x14ac:dyDescent="0.35">
@@ -2488,59 +2988,69 @@
         <v>14</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="9" t="s">
-        <v>77</v>
+      <c r="F10" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="7"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="7"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B13" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="B13" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
     </row>
     <row r="14" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="G16" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2555,30 +3065,32 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H9"/>
+  <dimension ref="B2:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
-    </row>
-    <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -2601,79 +3113,180 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>139</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E5" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="I5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>98</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>99</v>
+        <v>36</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="E6" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>109</v>
-      </c>
+      <c r="G6" s="2"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="9" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B9" s="7" t="s">
-        <v>110</v>
+    <row r="8" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="1">
+        <v>10</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2687,30 +3300,29 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H18"/>
+  <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
+      <c r="B2" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
@@ -2737,131 +3349,123 @@
     </row>
     <row r="4" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>99</v>
+        <v>140</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1">
         <v>6</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="E5" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>109</v>
+        <v>19</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>68</v>
+        <v>121</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>109</v>
-      </c>
+      <c r="G6" s="2"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
-        <v>109</v>
-      </c>
+      <c r="G7" s="2"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="1">
-        <v>10</v>
-      </c>
-      <c r="F8" s="9"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="7"/>
       <c r="G8" s="2"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="1">
         <v>10</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="9" t="s">
-        <v>77</v>
-      </c>
+      <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="9"/>
+      <c r="F11" s="7" t="s">
+        <v>76</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="1"/>
     </row>
@@ -2891,16 +3495,6 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="1"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
-        <v>104</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2913,30 +3507,30 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H21"/>
+  <dimension ref="B2:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:H8"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
+      <c r="B2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
@@ -2963,90 +3557,74 @@
     </row>
     <row r="4" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1">
         <v>6</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>119</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>120</v>
+        <v>44</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>90</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="1">
-        <v>10</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B8" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="17"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
@@ -3102,14 +3680,29 @@
       <c r="G14" s="2"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
-        <v>105</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -3123,28 +3716,30 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H10"/>
+  <dimension ref="B2:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
+      <c r="B2" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
@@ -3171,82 +3766,90 @@
     </row>
     <row r="4" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>86</v>
+        <v>157</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>143</v>
       </c>
       <c r="E4" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>109</v>
-      </c>
+      <c r="G4" s="2"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>143</v>
       </c>
       <c r="E5" s="1">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B6" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="D6" s="17" t="s">
+      <c r="B6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="9">
+        <v>20</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B7" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B8" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B7" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="17"/>
-    </row>
-    <row r="8" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="20"/>
+      <c r="C8" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
@@ -3265,6 +3868,21 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="1"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>156</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3277,32 +3895,31 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I18"/>
+  <dimension ref="B2:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
-    </row>
-    <row r="3" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -3325,34 +3942,36 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>98</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>80</v>
+        <v>143</v>
       </c>
       <c r="E4" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>147</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>44</v>
+        <v>148</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1">
         <v>20</v>
@@ -3361,53 +3980,48 @@
       <c r="G5" s="2"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>109</v>
-      </c>
+    <row r="6" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B6" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
       <c r="H6" s="1"/>
-      <c r="I6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B7" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -3416,7 +4030,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -3424,52 +4038,6 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E17" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E18" t="s">
-        <v>133</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3485,7 +4053,7 @@
   <dimension ref="B2:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:F11"/>
+      <selection activeCell="B10" sqref="B10:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
@@ -3496,15 +4064,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
@@ -3537,45 +4105,45 @@
         <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E5" s="1">
         <v>10</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -3592,7 +4160,7 @@
         <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E7" s="1">
         <v>5</v>
@@ -3614,7 +4182,7 @@
       <c r="E8" s="1">
         <v>300</v>
       </c>
-      <c r="F8" s="9"/>
+      <c r="F8" s="7"/>
       <c r="G8" s="2"/>
       <c r="H8" s="1"/>
     </row>

</xml_diff>